<commit_message>
added zipkin to moleculer appointments service
</commit_message>
<xml_diff>
--- a/Data/Implementation_Evaluation.xlsx
+++ b/Data/Implementation_Evaluation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\work\conferences\2020_ESSE\comparison\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32309862-4F52-4D80-9C10-E8137EAA01B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E7778D-1B15-4DDC-B220-CB59F4D55092}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>1.1 Distributed Configuration</t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>Moleculer</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>7. Automation</t>
@@ -883,7 +880,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15"/>
@@ -1000,8 +997,8 @@
       <c r="D6" s="14">
         <v>5</v>
       </c>
-      <c r="E6" s="14" t="s">
-        <v>32</v>
+      <c r="E6" s="14">
+        <v>5</v>
       </c>
       <c r="F6" s="14">
         <v>0</v>
@@ -1200,8 +1197,8 @@
       <c r="D18" s="16">
         <v>5</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>32</v>
+      <c r="E18" s="16">
+        <v>4</v>
       </c>
       <c r="F18" s="16">
         <v>0</v>
@@ -1220,8 +1217,8 @@
       <c r="D19" s="16">
         <v>5</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>32</v>
+      <c r="E19" s="16">
+        <v>5</v>
       </c>
       <c r="F19" s="16">
         <v>1</v>
@@ -1241,7 +1238,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F20" s="16">
         <v>1</v>
@@ -1249,7 +1246,7 @@
     </row>
     <row r="21" spans="1:6" ht="15.75">
       <c r="A21" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="16"/>
@@ -1259,7 +1256,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="16">
         <v>4</v>
@@ -1385,7 +1382,7 @@
       </c>
       <c r="E28" s="19">
         <f>SUM(E2:E27)</f>
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="F28" s="19">
         <f>SUM(F2:F27)</f>
@@ -1410,7 +1407,7 @@
       </c>
       <c r="E29" s="16">
         <f>E28/18</f>
-        <v>2.9444444444444446</v>
+        <v>3.9444444444444446</v>
       </c>
       <c r="F29" s="16">
         <f>F28/18</f>

</xml_diff>